<commit_message>
Fix VT field persistence and update modal window
- Fixed VT field handlers (date, start time, end time, availability) to properly persist data
- Changed VT field API calls from [fieldName] pattern to direct field names
- Added debug logging for VT field updates in backend
- Updated modal window to only show Description, Requirements, Steps, and Image
- Fixed backend Excel service to map Description field correctly
- Changed help button text from 'help' to 'Help'
- Added proper image handling with fallback text in modal
- All VT fields now persist correctly when refreshing the page
</commit_message>
<xml_diff>
--- a/backend/data/test_status.xlsx
+++ b/backend/data/test_status.xlsx
@@ -1222,10 +1222,10 @@
         <v>false</v>
       </c>
       <c r="Q11" t="str">
-        <v/>
+        <v>5467687</v>
       </c>
       <c r="R11" t="str">
-        <v/>
+        <v>2025-09-09</v>
       </c>
       <c r="S11" t="str">
         <v/>
@@ -1299,10 +1299,10 @@
         <v>false</v>
       </c>
       <c r="Q12" t="str">
-        <v/>
+        <v>6453</v>
       </c>
       <c r="R12" t="str">
-        <v/>
+        <v>2025-09-04</v>
       </c>
       <c r="S12" t="str">
         <v/>
@@ -1438,7 +1438,7 @@
         <v>All</v>
       </c>
       <c r="L14" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M14" t="str">
         <v>8/26/2025, 7:50:49 PM</v>
@@ -1592,7 +1592,7 @@
         <v>All</v>
       </c>
       <c r="L16" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M16" t="str">
         <v>8/26/2025, 7:50:49 PM</v>
@@ -1746,7 +1746,7 @@
         <v>All</v>
       </c>
       <c r="L18" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M18" t="str">
         <v>8/26/2025, 7:50:49 PM</v>
@@ -1900,7 +1900,7 @@
         <v>All</v>
       </c>
       <c r="L20" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M20" t="str">
         <v>8/26/2025, 7:50:49 PM</v>
@@ -2054,7 +2054,7 @@
         <v>All</v>
       </c>
       <c r="L22" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M22" t="str">
         <v>8/26/2025, 7:50:49 PM</v>
@@ -14990,7 +14990,7 @@
         <v>All</v>
       </c>
       <c r="L190" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M190" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15067,7 +15067,7 @@
         <v>All</v>
       </c>
       <c r="L191" t="str">
-        <v>NOT RUN</v>
+        <v>FAIL</v>
       </c>
       <c r="M191" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15144,7 +15144,7 @@
         <v>All</v>
       </c>
       <c r="L192" t="str">
-        <v>NOT RUN</v>
+        <v>BLOCKED</v>
       </c>
       <c r="M192" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15221,7 +15221,7 @@
         <v>First</v>
       </c>
       <c r="L193" t="str">
-        <v>NOT RUN</v>
+        <v>FAIL</v>
       </c>
       <c r="M193" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15298,7 +15298,7 @@
         <v>All</v>
       </c>
       <c r="L194" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M194" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15375,7 +15375,7 @@
         <v>All</v>
       </c>
       <c r="L195" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M195" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15452,7 +15452,7 @@
         <v>All</v>
       </c>
       <c r="L196" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M196" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15529,7 +15529,7 @@
         <v>All</v>
       </c>
       <c r="L197" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M197" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15606,7 +15606,7 @@
         <v>First</v>
       </c>
       <c r="L198" t="str">
-        <v>NOT RUN</v>
+        <v>FAIL</v>
       </c>
       <c r="M198" t="str">
         <v>9/3/2025, 3:51:43 PM</v>
@@ -15698,10 +15698,10 @@
         <v>false</v>
       </c>
       <c r="Q199" t="str">
-        <v/>
+        <v>78965446677</v>
       </c>
       <c r="R199" t="str">
-        <v/>
+        <v>2025-09-11</v>
       </c>
       <c r="S199" t="str">
         <v/>
@@ -15775,10 +15775,10 @@
         <v>false</v>
       </c>
       <c r="Q200" t="str">
-        <v/>
+        <v>569485798</v>
       </c>
       <c r="R200" t="str">
-        <v/>
+        <v>2025-09-08</v>
       </c>
       <c r="S200" t="str">
         <v/>
@@ -15852,10 +15852,10 @@
         <v>false</v>
       </c>
       <c r="Q201" t="str">
-        <v/>
+        <v>564765</v>
       </c>
       <c r="R201" t="str">
-        <v/>
+        <v>2025-09-10</v>
       </c>
       <c r="S201" t="str">
         <v/>
@@ -15914,13 +15914,13 @@
         <v>All</v>
       </c>
       <c r="L202" t="str">
-        <v>NOT RUN</v>
+        <v>FAIL</v>
       </c>
       <c r="M202" t="str">
-        <v>9/3/2025, 3:51:43 PM</v>
+        <v>9/9/2025, 12:50:44 PM</v>
       </c>
       <c r="N202" t="str">
-        <v/>
+        <v>Unknown</v>
       </c>
       <c r="O202" t="str">
         <v>Single Drive</v>
@@ -15935,16 +15935,16 @@
         <v/>
       </c>
       <c r="S202" t="str">
-        <v/>
+        <v>577848</v>
       </c>
       <c r="T202" t="str">
-        <v/>
+        <v>2025-09-08</v>
       </c>
       <c r="U202" t="str">
-        <v/>
+        <v>17:56</v>
       </c>
       <c r="V202" t="str">
-        <v/>
+        <v>19:59</v>
       </c>
       <c r="W202" t="str">
         <v/>
@@ -15953,7 +15953,7 @@
         <v/>
       </c>
       <c r="Y202" t="str">
-        <v/>
+        <v>dfrythyvr.  gevvtgtevgetrf</v>
       </c>
     </row>
     <row r="203">
@@ -15991,7 +15991,7 @@
         <v>All</v>
       </c>
       <c r="L203" t="str">
-        <v>NOT RUN</v>
+        <v>PASS</v>
       </c>
       <c r="M203" t="str">
         <v>9/3/2025, 3:51:43 PM</v>

</xml_diff>